<commit_message>
Income Analysis NO DEFLACTADO
</commit_message>
<xml_diff>
--- a/data_analysis/excels/Income Analysis ENCOVI 2014-2019.xlsx
+++ b/data_analysis/excels/Income Analysis ENCOVI 2014-2019.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wb546181\VEN\data_analysis\excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{341E4CCA-C554-4885-AF37-C57CE94D48B8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C167CB5-C006-4C41-9111-11542856F84D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -8247,8 +8247,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EBE7E7D-9185-4C55-876E-C79F0956F249}">
   <dimension ref="A1:O61"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="K37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="U65" sqref="U65"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="I1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="O22" sqref="O22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>